<commit_message>
Fix : update 'naver_wiki_total.xlsx' file
</commit_message>
<xml_diff>
--- a/Naver_Liquor_Wiki/naver_wiki_total.xlsx
+++ b/Naver_Liquor_Wiki/naver_wiki_total.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X1Carbon\Hee\ML_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591C27EF-C472-4EFB-9909-D0E472692D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CA6308-C2A8-48C7-9979-93CF94000CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1968" yWindow="-10296" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,9 +173,6 @@
     <t>귀감</t>
   </si>
   <si>
-    <t>그랑고또레드와인</t>
-  </si>
-  <si>
     <t>그랑꼬또로제와인</t>
   </si>
   <si>
@@ -921,9 +918,6 @@
   </si>
   <si>
     <t>오메기술</t>
-  </si>
-  <si>
-    <t>오메락퍽</t>
   </si>
   <si>
     <t>오미로제프리미어와인</t>
@@ -1720,6 +1714,14 @@
   </si>
   <si>
     <t>예천주복만월40</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>오매락퍽</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>그랑꼬또레드와인</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2162,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J534"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="L332" sqref="L332"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -2173,7 +2175,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2326,7 +2328,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2343,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -2366,7 +2368,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D10">
         <v>4</v>
@@ -2543,7 +2545,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -2597,7 +2599,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -2725,7 +2727,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -2762,7 +2764,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2782,7 +2784,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -2799,7 +2801,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C33">
         <v>3</v>
@@ -2816,7 +2818,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -2833,7 +2835,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C35">
         <v>3</v>
@@ -2967,7 +2969,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C42">
         <v>3</v>
@@ -2984,7 +2986,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C43">
         <v>4</v>
@@ -3138,7 +3140,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>541</v>
       </c>
       <c r="D51">
         <v>3</v>
@@ -3158,7 +3160,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -3178,7 +3180,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D53">
         <v>4</v>
@@ -3198,7 +3200,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -3218,7 +3220,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -3238,7 +3240,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D56">
         <v>3</v>
@@ -3258,7 +3260,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D57">
         <v>3</v>
@@ -3278,7 +3280,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -3298,7 +3300,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -3318,7 +3320,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -3338,7 +3340,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C61">
         <v>4</v>
@@ -3355,7 +3357,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C62">
         <v>4</v>
@@ -3372,7 +3374,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D63">
         <v>3</v>
@@ -3392,7 +3394,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D64">
         <v>3</v>
@@ -3412,7 +3414,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -3432,7 +3434,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -3452,7 +3454,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D67">
         <v>2</v>
@@ -3472,7 +3474,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D68">
         <v>2</v>
@@ -3492,7 +3494,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -3512,7 +3514,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D70">
         <v>4</v>
@@ -3532,7 +3534,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -3552,7 +3554,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -3569,7 +3571,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -3589,7 +3591,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D74">
         <v>3</v>
@@ -3609,7 +3611,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -3629,7 +3631,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -3649,7 +3651,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D77">
         <v>4</v>
@@ -3669,7 +3671,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D78">
         <v>3</v>
@@ -3689,7 +3691,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D79">
         <v>4</v>
@@ -3709,7 +3711,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D80">
         <v>3</v>
@@ -3729,7 +3731,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D81">
         <v>3</v>
@@ -3749,7 +3751,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D82">
         <v>3</v>
@@ -3769,7 +3771,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -3789,7 +3791,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -3806,7 +3808,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -3823,7 +3825,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D86">
         <v>4</v>
@@ -3843,7 +3845,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D87">
         <v>4</v>
@@ -3863,7 +3865,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D88">
         <v>3</v>
@@ -3883,7 +3885,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D89">
         <v>4</v>
@@ -3903,7 +3905,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D90">
         <v>3</v>
@@ -3923,7 +3925,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D91">
         <v>1</v>
@@ -3943,7 +3945,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -3963,7 +3965,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -3983,7 +3985,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -4003,7 +4005,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -4023,7 +4025,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -4043,7 +4045,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -4063,7 +4065,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D98">
         <v>1</v>
@@ -4083,7 +4085,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D99">
         <v>3</v>
@@ -4103,7 +4105,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C100">
         <v>4</v>
@@ -4120,7 +4122,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D101">
         <v>3</v>
@@ -4140,7 +4142,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D102">
         <v>4</v>
@@ -4160,7 +4162,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -4180,7 +4182,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D104">
         <v>2</v>
@@ -4200,7 +4202,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D105">
         <v>2</v>
@@ -4220,7 +4222,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D106">
         <v>1</v>
@@ -4240,7 +4242,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D107">
         <v>4</v>
@@ -4260,7 +4262,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -4280,7 +4282,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D109">
         <v>2</v>
@@ -4300,7 +4302,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D110">
         <v>4</v>
@@ -4320,7 +4322,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D111">
         <v>3</v>
@@ -4340,7 +4342,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D112">
         <v>3</v>
@@ -4360,7 +4362,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D113">
         <v>4</v>
@@ -4380,7 +4382,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D114">
         <v>1</v>
@@ -4400,7 +4402,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C115">
         <v>2</v>
@@ -4417,7 +4419,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C116">
         <v>3</v>
@@ -4434,7 +4436,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D117">
         <v>2</v>
@@ -4454,7 +4456,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D118">
         <v>4</v>
@@ -4474,7 +4476,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C119" s="2"/>
       <c r="D119" s="2">
@@ -4495,7 +4497,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D120">
         <v>3</v>
@@ -4515,7 +4517,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D121">
         <v>2</v>
@@ -4535,7 +4537,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -4552,7 +4554,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C123">
         <v>4</v>
@@ -4569,7 +4571,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D124">
         <v>2</v>
@@ -4589,7 +4591,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C125">
         <v>2</v>
@@ -4606,7 +4608,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C126">
         <v>3</v>
@@ -4623,7 +4625,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D127">
         <v>2</v>
@@ -4643,7 +4645,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D128">
         <v>3</v>
@@ -4663,7 +4665,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D129">
         <v>3</v>
@@ -4683,7 +4685,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D130">
         <v>3</v>
@@ -4703,7 +4705,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D131">
         <v>3</v>
@@ -4723,7 +4725,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C132">
         <v>3</v>
@@ -4740,7 +4742,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C133">
         <v>2</v>
@@ -4757,7 +4759,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C134">
         <v>2</v>
@@ -4774,7 +4776,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C135">
         <v>1</v>
@@ -4791,7 +4793,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C136">
         <v>4</v>
@@ -4808,7 +4810,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D137">
         <v>3</v>
@@ -4828,7 +4830,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D138">
         <v>4</v>
@@ -4848,7 +4850,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C139">
         <v>3</v>
@@ -4865,7 +4867,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C140">
         <v>4</v>
@@ -4882,7 +4884,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D141">
         <v>2</v>
@@ -4902,7 +4904,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D142">
         <v>3</v>
@@ -4922,7 +4924,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D143">
         <v>3</v>
@@ -4942,7 +4944,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D144">
         <v>3</v>
@@ -4962,7 +4964,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D145">
         <v>3</v>
@@ -4982,7 +4984,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D146">
         <v>3</v>
@@ -5002,7 +5004,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D147">
         <v>3</v>
@@ -5022,7 +5024,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C148">
         <v>2</v>
@@ -5039,7 +5041,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D149">
         <v>3</v>
@@ -5059,7 +5061,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D150">
         <v>3</v>
@@ -5079,7 +5081,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D151">
         <v>2</v>
@@ -5099,7 +5101,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D152">
         <v>4</v>
@@ -5119,7 +5121,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D153">
         <v>4</v>
@@ -5139,7 +5141,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C154">
         <v>3</v>
@@ -5156,7 +5158,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D155">
         <v>3</v>
@@ -5176,7 +5178,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D156">
         <v>3</v>
@@ -5193,7 +5195,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C157">
         <v>2</v>
@@ -5210,7 +5212,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -5227,7 +5229,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -5244,7 +5246,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C160">
         <v>1</v>
@@ -5261,7 +5263,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D161">
         <v>1</v>
@@ -5281,7 +5283,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D162">
         <v>3</v>
@@ -5301,7 +5303,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C163">
         <v>3</v>
@@ -5318,7 +5320,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C164">
         <v>3</v>
@@ -5335,7 +5337,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D165">
         <v>1</v>
@@ -5355,7 +5357,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C166">
         <v>4</v>
@@ -5372,7 +5374,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D167">
         <v>1</v>
@@ -5392,7 +5394,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C168">
         <v>3</v>
@@ -5409,7 +5411,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D169">
         <v>4</v>
@@ -5429,7 +5431,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D170">
         <v>2</v>
@@ -5449,7 +5451,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D171">
         <v>2</v>
@@ -5469,7 +5471,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C172">
         <v>3</v>
@@ -5486,7 +5488,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C173">
         <v>3</v>
@@ -5503,7 +5505,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C174">
         <v>4</v>
@@ -5520,7 +5522,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D175">
         <v>2</v>
@@ -5540,7 +5542,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C176">
         <v>2</v>
@@ -5557,7 +5559,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C177">
         <v>2</v>
@@ -5574,7 +5576,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C178">
         <v>2</v>
@@ -5591,7 +5593,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D179">
         <v>3</v>
@@ -5611,7 +5613,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D180">
         <v>3</v>
@@ -5631,7 +5633,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D181">
         <v>2</v>
@@ -5651,7 +5653,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D182">
         <v>1</v>
@@ -5671,7 +5673,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D183">
         <v>2</v>
@@ -5691,7 +5693,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D184">
         <v>3</v>
@@ -5711,7 +5713,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D185">
         <v>4</v>
@@ -5731,7 +5733,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D186">
         <v>4</v>
@@ -5751,7 +5753,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D187">
         <v>3</v>
@@ -5771,7 +5773,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -5788,7 +5790,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D189">
         <v>4</v>
@@ -5808,7 +5810,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D190">
         <v>5</v>
@@ -5828,7 +5830,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D191">
         <v>2</v>
@@ -5848,7 +5850,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D192">
         <v>2</v>
@@ -5868,7 +5870,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D193">
         <v>3</v>
@@ -5888,7 +5890,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C194">
         <v>4</v>
@@ -5908,7 +5910,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C195">
         <v>2</v>
@@ -5925,7 +5927,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D196">
         <v>3</v>
@@ -5945,7 +5947,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D197">
         <v>2</v>
@@ -5965,7 +5967,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D198">
         <v>2</v>
@@ -5985,7 +5987,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D199">
         <v>2</v>
@@ -6005,7 +6007,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D200">
         <v>2</v>
@@ -6025,7 +6027,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D201">
         <v>3</v>
@@ -6045,7 +6047,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D202">
         <v>2</v>
@@ -6065,7 +6067,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D203">
         <v>3</v>
@@ -6085,7 +6087,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D204">
         <v>3</v>
@@ -6105,7 +6107,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D205">
         <v>4</v>
@@ -6125,7 +6127,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D206">
         <v>5</v>
@@ -6145,7 +6147,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D207">
         <v>4</v>
@@ -6165,7 +6167,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D208">
         <v>3</v>
@@ -6185,7 +6187,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D209">
         <v>2</v>
@@ -6205,7 +6207,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D210">
         <v>4</v>
@@ -6225,7 +6227,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D211">
         <v>2</v>
@@ -6245,7 +6247,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D212">
         <v>3</v>
@@ -6265,7 +6267,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C213">
         <v>4</v>
@@ -6282,7 +6284,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D214">
         <v>3</v>
@@ -6302,7 +6304,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C215">
         <v>3</v>
@@ -6319,7 +6321,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D216">
         <v>2</v>
@@ -6339,7 +6341,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D217">
         <v>2</v>
@@ -6359,7 +6361,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D218">
         <v>1</v>
@@ -6379,7 +6381,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D219">
         <v>1</v>
@@ -6399,7 +6401,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D220">
         <v>1</v>
@@ -6419,7 +6421,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D221">
         <v>2</v>
@@ -6439,7 +6441,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D222">
         <v>3</v>
@@ -6459,7 +6461,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D223">
         <v>4</v>
@@ -6479,7 +6481,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C224">
         <v>3</v>
@@ -6496,7 +6498,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D225">
         <v>4</v>
@@ -6516,7 +6518,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D226">
         <v>3</v>
@@ -6536,7 +6538,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D227">
         <v>4</v>
@@ -6556,7 +6558,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D228">
         <v>4</v>
@@ -6576,7 +6578,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D229">
         <v>2</v>
@@ -6596,7 +6598,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D230">
         <v>3</v>
@@ -6616,7 +6618,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D231">
         <v>1</v>
@@ -6636,7 +6638,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D232">
         <v>1</v>
@@ -6656,7 +6658,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D233">
         <v>2</v>
@@ -6676,7 +6678,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D234">
         <v>2</v>
@@ -6696,7 +6698,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D235">
         <v>3</v>
@@ -6716,7 +6718,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D236">
         <v>4</v>
@@ -6736,7 +6738,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D237">
         <v>2</v>
@@ -6756,7 +6758,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D238">
         <v>3</v>
@@ -6776,7 +6778,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D239">
         <v>3</v>
@@ -6796,7 +6798,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C240">
         <v>3</v>
@@ -6813,7 +6815,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D241">
         <v>4</v>
@@ -6833,7 +6835,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C242">
         <v>4</v>
@@ -6850,7 +6852,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D243">
         <v>3</v>
@@ -6870,7 +6872,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D244">
         <v>1</v>
@@ -6890,7 +6892,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D245">
         <v>1</v>
@@ -6910,7 +6912,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D246">
         <v>2</v>
@@ -6930,7 +6932,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D247">
         <v>4</v>
@@ -6950,7 +6952,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D248">
         <v>4</v>
@@ -6970,7 +6972,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D249">
         <v>4</v>
@@ -6990,7 +6992,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D250">
         <v>2</v>
@@ -7010,7 +7012,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D251">
         <v>2</v>
@@ -7030,7 +7032,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C252">
         <v>2</v>
@@ -7047,7 +7049,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C253">
         <v>1</v>
@@ -7064,7 +7066,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D254">
         <v>2</v>
@@ -7084,7 +7086,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D255">
         <v>2</v>
@@ -7104,7 +7106,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D256">
         <v>3</v>
@@ -7124,7 +7126,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D257">
         <v>3</v>
@@ -7144,7 +7146,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C258">
         <v>5</v>
@@ -7161,7 +7163,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D259">
         <v>3</v>
@@ -7181,7 +7183,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D260">
         <v>3</v>
@@ -7201,7 +7203,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D261">
         <v>3</v>
@@ -7221,7 +7223,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D262">
         <v>4</v>
@@ -7241,7 +7243,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D263">
         <v>1</v>
@@ -7261,7 +7263,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D264">
         <v>2</v>
@@ -7281,7 +7283,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C265">
         <v>3</v>
@@ -7298,7 +7300,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D266">
         <v>3</v>
@@ -7318,7 +7320,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D267">
         <v>2</v>
@@ -7338,7 +7340,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D268">
         <v>2</v>
@@ -7358,7 +7360,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D269">
         <v>1</v>
@@ -7378,7 +7380,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D270">
         <v>2</v>
@@ -7398,7 +7400,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D271">
         <v>1</v>
@@ -7418,7 +7420,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D272">
         <v>2</v>
@@ -7438,7 +7440,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D273">
         <v>1</v>
@@ -7458,7 +7460,7 @@
         <v>272</v>
       </c>
       <c r="B274" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D274">
         <v>1</v>
@@ -7478,7 +7480,7 @@
         <v>273</v>
       </c>
       <c r="B275" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F275">
         <v>3</v>
@@ -7495,7 +7497,7 @@
         <v>274</v>
       </c>
       <c r="B276" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D276">
         <v>2</v>
@@ -7515,7 +7517,7 @@
         <v>275</v>
       </c>
       <c r="B277" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D277">
         <v>3</v>
@@ -7535,7 +7537,7 @@
         <v>276</v>
       </c>
       <c r="B278" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D278">
         <v>2</v>
@@ -7555,7 +7557,7 @@
         <v>277</v>
       </c>
       <c r="B279" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D279">
         <v>4</v>
@@ -7575,7 +7577,7 @@
         <v>278</v>
       </c>
       <c r="B280" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D280">
         <v>4</v>
@@ -7595,7 +7597,7 @@
         <v>279</v>
       </c>
       <c r="B281" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D281">
         <v>3</v>
@@ -7615,7 +7617,7 @@
         <v>280</v>
       </c>
       <c r="B282" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D282">
         <v>5</v>
@@ -7635,7 +7637,7 @@
         <v>281</v>
       </c>
       <c r="B283" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D283">
         <v>5</v>
@@ -7655,7 +7657,7 @@
         <v>282</v>
       </c>
       <c r="B284" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D284">
         <v>5</v>
@@ -7675,7 +7677,7 @@
         <v>283</v>
       </c>
       <c r="B285" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D285">
         <v>1</v>
@@ -7695,7 +7697,7 @@
         <v>284</v>
       </c>
       <c r="B286" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D286">
         <v>4</v>
@@ -7715,7 +7717,7 @@
         <v>285</v>
       </c>
       <c r="B287" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D287">
         <v>2</v>
@@ -7735,7 +7737,7 @@
         <v>286</v>
       </c>
       <c r="B288" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D288">
         <v>3</v>
@@ -7755,7 +7757,7 @@
         <v>287</v>
       </c>
       <c r="B289" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D289">
         <v>3</v>
@@ -7775,7 +7777,7 @@
         <v>288</v>
       </c>
       <c r="B290" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D290">
         <v>2</v>
@@ -7795,7 +7797,7 @@
         <v>289</v>
       </c>
       <c r="B291" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D291">
         <v>3</v>
@@ -7815,7 +7817,7 @@
         <v>290</v>
       </c>
       <c r="B292" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D292">
         <v>3</v>
@@ -7835,7 +7837,7 @@
         <v>291</v>
       </c>
       <c r="B293" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D293">
         <v>2</v>
@@ -7855,7 +7857,7 @@
         <v>292</v>
       </c>
       <c r="B294" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D294">
         <v>3</v>
@@ -7875,7 +7877,7 @@
         <v>293</v>
       </c>
       <c r="B295" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D295">
         <v>4</v>
@@ -7895,7 +7897,7 @@
         <v>294</v>
       </c>
       <c r="B296" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D296">
         <v>2</v>
@@ -7915,7 +7917,7 @@
         <v>295</v>
       </c>
       <c r="B297" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F297">
         <v>4</v>
@@ -7932,7 +7934,7 @@
         <v>296</v>
       </c>
       <c r="B298" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D298">
         <v>3</v>
@@ -7952,7 +7954,7 @@
         <v>297</v>
       </c>
       <c r="B299" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D299">
         <v>2</v>
@@ -7975,7 +7977,7 @@
         <v>298</v>
       </c>
       <c r="B300" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D300">
         <v>3</v>
@@ -7995,7 +7997,7 @@
         <v>299</v>
       </c>
       <c r="B301" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C301">
         <v>4</v>
@@ -8015,7 +8017,7 @@
         <v>300</v>
       </c>
       <c r="B302" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C302">
         <v>4</v>
@@ -8038,7 +8040,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D303">
         <v>3</v>
@@ -8058,7 +8060,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D304">
         <v>3</v>
@@ -8078,7 +8080,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D305">
         <v>1</v>
@@ -8098,7 +8100,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C306">
         <v>2</v>
@@ -8115,7 +8117,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C307">
         <v>3</v>
@@ -8132,7 +8134,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C308">
         <v>1</v>
@@ -8149,7 +8151,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C309">
         <v>1</v>
@@ -8166,7 +8168,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C310">
         <v>1</v>
@@ -8183,7 +8185,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C311">
         <v>3</v>
@@ -8200,7 +8202,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D312">
         <v>3</v>
@@ -8220,7 +8222,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D313">
         <v>3</v>
@@ -8240,7 +8242,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D314">
         <v>4</v>
@@ -8260,7 +8262,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D315">
         <v>4</v>
@@ -8280,7 +8282,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D316">
         <v>4</v>
@@ -8300,7 +8302,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D317">
         <v>4</v>
@@ -8320,7 +8322,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D318">
         <v>1</v>
@@ -8340,7 +8342,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D319">
         <v>2</v>
@@ -8360,7 +8362,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D320">
         <v>2</v>
@@ -8380,7 +8382,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C321">
         <v>2</v>
@@ -8397,7 +8399,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C322">
         <v>3</v>
@@ -8414,7 +8416,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D323">
         <v>2</v>
@@ -8434,7 +8436,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D324">
         <v>4</v>
@@ -8454,7 +8456,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D325">
         <v>1</v>
@@ -8474,7 +8476,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D326">
         <v>2</v>
@@ -8494,7 +8496,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D327">
         <v>2</v>
@@ -8514,7 +8516,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C328">
         <v>3</v>
@@ -8531,7 +8533,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D329">
         <v>2</v>
@@ -8551,7 +8553,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D330">
         <v>4</v>
@@ -8571,7 +8573,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C331">
         <v>2</v>
@@ -8588,7 +8590,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D332">
         <v>1</v>
@@ -8608,7 +8610,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D333">
         <v>1</v>
@@ -8628,7 +8630,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D334">
         <v>4</v>
@@ -8648,7 +8650,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D335">
         <v>1</v>
@@ -8668,7 +8670,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C336">
         <v>3</v>
@@ -8685,7 +8687,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C337">
         <v>4</v>
@@ -8702,7 +8704,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C338">
         <v>3</v>
@@ -8719,7 +8721,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C339">
         <v>3</v>
@@ -8736,7 +8738,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D340">
         <v>2</v>
@@ -8776,7 +8778,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D342">
         <v>3</v>
@@ -8796,7 +8798,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D343">
         <v>5</v>
@@ -8816,7 +8818,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D344">
         <v>1</v>
@@ -8836,7 +8838,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D345">
         <v>2</v>
@@ -8856,7 +8858,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="s">
-        <v>295</v>
+        <v>540</v>
       </c>
       <c r="C346">
         <v>3</v>
@@ -8873,7 +8875,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D347">
         <v>2</v>
@@ -8893,7 +8895,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D348">
         <v>3</v>
@@ -8913,7 +8915,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D349">
         <v>1</v>
@@ -8933,7 +8935,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D350">
         <v>2</v>
@@ -8953,7 +8955,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D351">
         <v>1</v>
@@ -8973,7 +8975,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C352">
         <v>3</v>
@@ -8990,7 +8992,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D353">
         <v>3</v>
@@ -9010,7 +9012,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D354">
         <v>4</v>
@@ -9030,7 +9032,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D355">
         <v>4</v>
@@ -9050,7 +9052,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D356">
         <v>4</v>
@@ -9070,7 +9072,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D357">
         <v>3</v>
@@ -9090,7 +9092,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C358">
         <v>4</v>
@@ -9107,7 +9109,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C359">
         <v>3</v>
@@ -9124,7 +9126,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="C360">
         <v>3</v>
@@ -9141,7 +9143,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D361">
         <v>3</v>
@@ -9161,7 +9163,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D362">
         <v>2</v>
@@ -9181,7 +9183,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D363">
         <v>3</v>
@@ -9201,7 +9203,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D364">
         <v>2</v>
@@ -9221,7 +9223,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D365">
         <v>2</v>
@@ -9241,7 +9243,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D366">
         <v>2</v>
@@ -9261,7 +9263,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D367">
         <v>2</v>
@@ -9281,7 +9283,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D368">
         <v>1</v>
@@ -9301,7 +9303,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D369">
         <v>1</v>
@@ -9321,7 +9323,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D370">
         <v>2</v>
@@ -9341,7 +9343,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D371">
         <v>2</v>
@@ -9361,7 +9363,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C372">
         <v>2</v>
@@ -9384,7 +9386,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D373">
         <v>1</v>
@@ -9404,7 +9406,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D374">
         <v>3</v>
@@ -9424,7 +9426,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D375">
         <v>3</v>
@@ -9444,7 +9446,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D376">
         <v>2</v>
@@ -9464,7 +9466,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D377">
         <v>3</v>
@@ -9484,7 +9486,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D378">
         <v>1</v>
@@ -9504,7 +9506,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D379">
         <v>2</v>
@@ -9524,7 +9526,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D380">
         <v>2</v>
@@ -9544,7 +9546,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D381">
         <v>2</v>
@@ -9564,7 +9566,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D382">
         <v>2</v>
@@ -9584,7 +9586,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C383">
         <v>1</v>
@@ -9601,7 +9603,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D384">
         <v>1</v>
@@ -9621,7 +9623,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D385">
         <v>2</v>
@@ -9641,7 +9643,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D386">
         <v>2</v>
@@ -9661,7 +9663,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D387">
         <v>2</v>
@@ -9681,7 +9683,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D388">
         <v>3</v>
@@ -9701,7 +9703,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D389">
         <v>1</v>
@@ -9721,7 +9723,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D390">
         <v>4</v>
@@ -9741,7 +9743,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D391">
         <v>4</v>
@@ -9761,7 +9763,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D392">
         <v>3</v>
@@ -9781,7 +9783,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D393">
         <v>3</v>
@@ -9801,7 +9803,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C394">
         <v>4</v>
@@ -9818,7 +9820,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D395">
         <v>2</v>
@@ -9838,7 +9840,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D396">
         <v>3</v>
@@ -9858,7 +9860,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D397">
         <v>1</v>
@@ -9878,7 +9880,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D398">
         <v>3</v>
@@ -9898,7 +9900,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D399">
         <v>3</v>
@@ -9918,7 +9920,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D400">
         <v>3</v>
@@ -9938,7 +9940,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D401">
         <v>2</v>
@@ -9958,7 +9960,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D402">
         <v>5</v>
@@ -9978,7 +9980,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C403">
         <v>4</v>
@@ -9995,7 +9997,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D404">
         <v>1</v>
@@ -10015,7 +10017,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D405">
         <v>2</v>
@@ -10035,7 +10037,7 @@
         <v>404</v>
       </c>
       <c r="B406" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D406">
         <v>4</v>
@@ -10058,7 +10060,7 @@
         <v>405</v>
       </c>
       <c r="B407" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D407">
         <v>4</v>
@@ -10078,7 +10080,7 @@
         <v>406</v>
       </c>
       <c r="B408" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D408">
         <v>4</v>
@@ -10101,7 +10103,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D409">
         <v>1</v>
@@ -10121,7 +10123,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D410">
         <v>1</v>
@@ -10141,7 +10143,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D411">
         <v>3</v>
@@ -10161,7 +10163,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D412">
         <v>2</v>
@@ -10181,7 +10183,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D413">
         <v>3</v>
@@ -10201,7 +10203,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D414">
         <v>4</v>
@@ -10221,7 +10223,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D415">
         <v>4</v>
@@ -10241,7 +10243,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C416">
         <v>3</v>
@@ -10258,7 +10260,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C417">
         <v>3</v>
@@ -10275,7 +10277,7 @@
         <v>416</v>
       </c>
       <c r="B418" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C418">
         <v>4</v>
@@ -10292,7 +10294,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C419">
         <v>4</v>
@@ -10309,7 +10311,7 @@
         <v>418</v>
       </c>
       <c r="B420" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D420">
         <v>1</v>
@@ -10329,7 +10331,7 @@
         <v>419</v>
       </c>
       <c r="B421" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D421">
         <v>1</v>
@@ -10349,7 +10351,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D422">
         <v>3</v>
@@ -10369,7 +10371,7 @@
         <v>421</v>
       </c>
       <c r="B423" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C423">
         <v>3</v>
@@ -10386,7 +10388,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D424">
         <v>2</v>
@@ -10406,7 +10408,7 @@
         <v>423</v>
       </c>
       <c r="B425" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D425">
         <v>3</v>
@@ -10426,7 +10428,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D426">
         <v>2</v>
@@ -10446,7 +10448,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D427">
         <v>1</v>
@@ -10466,7 +10468,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C428">
         <v>2</v>
@@ -10483,7 +10485,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D429">
         <v>3</v>
@@ -10503,7 +10505,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C430">
         <v>2</v>
@@ -10520,7 +10522,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D431">
         <v>2</v>
@@ -10540,7 +10542,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C432">
         <v>3</v>
@@ -10557,7 +10559,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D433">
         <v>2</v>
@@ -10577,7 +10579,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D434">
         <v>2</v>
@@ -10597,7 +10599,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C435">
         <v>5</v>
@@ -10614,7 +10616,7 @@
         <v>434</v>
       </c>
       <c r="B436" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D436">
         <v>2</v>
@@ -10634,7 +10636,7 @@
         <v>435</v>
       </c>
       <c r="B437" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D437">
         <v>3</v>
@@ -10654,7 +10656,7 @@
         <v>436</v>
       </c>
       <c r="B438" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D438">
         <v>3</v>
@@ -10674,7 +10676,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D439">
         <v>4</v>
@@ -10694,7 +10696,7 @@
         <v>438</v>
       </c>
       <c r="B440" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D440">
         <v>1</v>
@@ -10714,7 +10716,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D441">
         <v>2</v>
@@ -10734,7 +10736,7 @@
         <v>440</v>
       </c>
       <c r="B442" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D442">
         <v>1</v>
@@ -10754,7 +10756,7 @@
         <v>441</v>
       </c>
       <c r="B443" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D443">
         <v>3</v>
@@ -10774,7 +10776,7 @@
         <v>442</v>
       </c>
       <c r="B444" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D444">
         <v>2</v>
@@ -10794,7 +10796,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D445">
         <v>2</v>
@@ -10814,7 +10816,7 @@
         <v>444</v>
       </c>
       <c r="B446" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D446">
         <v>3</v>
@@ -10834,7 +10836,7 @@
         <v>445</v>
       </c>
       <c r="B447" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D447">
         <v>2</v>
@@ -10854,7 +10856,7 @@
         <v>446</v>
       </c>
       <c r="B448" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D448">
         <v>2</v>
@@ -10874,7 +10876,7 @@
         <v>447</v>
       </c>
       <c r="B449" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D449">
         <v>1</v>
@@ -10894,7 +10896,7 @@
         <v>448</v>
       </c>
       <c r="B450" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C450">
         <v>5</v>
@@ -10911,7 +10913,7 @@
         <v>449</v>
       </c>
       <c r="B451" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D451">
         <v>2</v>
@@ -10931,7 +10933,7 @@
         <v>450</v>
       </c>
       <c r="B452" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C452">
         <v>4</v>
@@ -10954,7 +10956,7 @@
         <v>451</v>
       </c>
       <c r="B453" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D453">
         <v>3</v>
@@ -10974,7 +10976,7 @@
         <v>452</v>
       </c>
       <c r="B454" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D454">
         <v>3</v>
@@ -10994,7 +10996,7 @@
         <v>453</v>
       </c>
       <c r="B455" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D455">
         <v>2</v>
@@ -11014,7 +11016,7 @@
         <v>454</v>
       </c>
       <c r="B456" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D456">
         <v>3</v>
@@ -11034,7 +11036,7 @@
         <v>455</v>
       </c>
       <c r="B457" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C457">
         <v>4</v>
@@ -11051,7 +11053,7 @@
         <v>456</v>
       </c>
       <c r="B458" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D458">
         <v>1</v>
@@ -11071,7 +11073,7 @@
         <v>457</v>
       </c>
       <c r="B459" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D459">
         <v>2</v>
@@ -11091,7 +11093,7 @@
         <v>458</v>
       </c>
       <c r="B460" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D460">
         <v>3</v>
@@ -11111,7 +11113,7 @@
         <v>459</v>
       </c>
       <c r="B461" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D461">
         <v>3</v>
@@ -11131,7 +11133,7 @@
         <v>460</v>
       </c>
       <c r="B462" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D462">
         <v>2</v>
@@ -11151,7 +11153,7 @@
         <v>461</v>
       </c>
       <c r="B463" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D463">
         <v>1</v>
@@ -11171,7 +11173,7 @@
         <v>462</v>
       </c>
       <c r="B464" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D464">
         <v>3</v>
@@ -11191,7 +11193,7 @@
         <v>463</v>
       </c>
       <c r="B465" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D465">
         <v>2</v>
@@ -11211,7 +11213,7 @@
         <v>464</v>
       </c>
       <c r="B466" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D466">
         <v>4</v>
@@ -11231,7 +11233,7 @@
         <v>465</v>
       </c>
       <c r="B467" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D467">
         <v>4</v>
@@ -11251,7 +11253,7 @@
         <v>466</v>
       </c>
       <c r="B468" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D468">
         <v>1</v>
@@ -11271,7 +11273,7 @@
         <v>467</v>
       </c>
       <c r="B469" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D469">
         <v>4</v>
@@ -11291,7 +11293,7 @@
         <v>468</v>
       </c>
       <c r="B470" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C470">
         <v>3</v>
@@ -11308,7 +11310,7 @@
         <v>469</v>
       </c>
       <c r="B471" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C471">
         <v>2</v>
@@ -11325,7 +11327,7 @@
         <v>470</v>
       </c>
       <c r="B472" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C472">
         <v>4</v>
@@ -11342,7 +11344,7 @@
         <v>471</v>
       </c>
       <c r="B473" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D473">
         <v>3</v>
@@ -11362,7 +11364,7 @@
         <v>472</v>
       </c>
       <c r="B474" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D474">
         <v>3</v>
@@ -11382,7 +11384,7 @@
         <v>473</v>
       </c>
       <c r="B475" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D475">
         <v>3</v>
@@ -11402,7 +11404,7 @@
         <v>474</v>
       </c>
       <c r="B476" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D476">
         <v>3</v>
@@ -11422,7 +11424,7 @@
         <v>475</v>
       </c>
       <c r="B477" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D477">
         <v>1</v>
@@ -11442,7 +11444,7 @@
         <v>476</v>
       </c>
       <c r="B478" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D478">
         <v>1</v>
@@ -11462,7 +11464,7 @@
         <v>477</v>
       </c>
       <c r="B479" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D479">
         <v>2</v>
@@ -11482,7 +11484,7 @@
         <v>478</v>
       </c>
       <c r="B480" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D480">
         <v>4</v>
@@ -11502,7 +11504,7 @@
         <v>479</v>
       </c>
       <c r="B481" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D481">
         <v>4</v>
@@ -11522,7 +11524,7 @@
         <v>480</v>
       </c>
       <c r="B482" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D482">
         <v>4</v>
@@ -11542,7 +11544,7 @@
         <v>481</v>
       </c>
       <c r="B483" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D483">
         <v>2</v>
@@ -11562,7 +11564,7 @@
         <v>482</v>
       </c>
       <c r="B484" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C484">
         <v>3</v>
@@ -11579,7 +11581,7 @@
         <v>483</v>
       </c>
       <c r="B485" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D485">
         <v>1</v>
@@ -11599,7 +11601,7 @@
         <v>484</v>
       </c>
       <c r="B486" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D486">
         <v>2</v>
@@ -11619,7 +11621,7 @@
         <v>485</v>
       </c>
       <c r="B487" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D487">
         <v>4</v>
@@ -11639,7 +11641,7 @@
         <v>486</v>
       </c>
       <c r="B488" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D488">
         <v>3</v>
@@ -11659,7 +11661,7 @@
         <v>487</v>
       </c>
       <c r="B489" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C489">
         <v>3</v>
@@ -11676,7 +11678,7 @@
         <v>488</v>
       </c>
       <c r="B490" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C490">
         <v>4</v>
@@ -11693,7 +11695,7 @@
         <v>489</v>
       </c>
       <c r="B491" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C491">
         <v>5</v>
@@ -11710,7 +11712,7 @@
         <v>490</v>
       </c>
       <c r="B492" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C492">
         <v>2</v>
@@ -11727,7 +11729,7 @@
         <v>491</v>
       </c>
       <c r="B493" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C493">
         <v>2</v>
@@ -11744,7 +11746,7 @@
         <v>492</v>
       </c>
       <c r="B494" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D494">
         <v>3</v>
@@ -11764,7 +11766,7 @@
         <v>493</v>
       </c>
       <c r="B495" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D495">
         <v>4</v>
@@ -11784,7 +11786,7 @@
         <v>494</v>
       </c>
       <c r="B496" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C496">
         <v>4</v>
@@ -11801,7 +11803,7 @@
         <v>495</v>
       </c>
       <c r="B497" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C497">
         <v>3</v>
@@ -11818,7 +11820,7 @@
         <v>496</v>
       </c>
       <c r="B498" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D498">
         <v>3</v>
@@ -11838,7 +11840,7 @@
         <v>497</v>
       </c>
       <c r="B499" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D499">
         <v>5</v>
@@ -11858,7 +11860,7 @@
         <v>498</v>
       </c>
       <c r="B500" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D500">
         <v>3</v>
@@ -11878,7 +11880,7 @@
         <v>499</v>
       </c>
       <c r="B501" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D501">
         <v>3</v>
@@ -11898,7 +11900,7 @@
         <v>500</v>
       </c>
       <c r="B502" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C502">
         <v>2</v>
@@ -11915,7 +11917,7 @@
         <v>501</v>
       </c>
       <c r="B503" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C503">
         <v>3</v>
@@ -11932,7 +11934,7 @@
         <v>502</v>
       </c>
       <c r="B504" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D504">
         <v>1</v>
@@ -11952,7 +11954,7 @@
         <v>503</v>
       </c>
       <c r="B505" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D505">
         <v>1</v>
@@ -11972,7 +11974,7 @@
         <v>504</v>
       </c>
       <c r="B506" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D506">
         <v>1</v>
@@ -11992,7 +11994,7 @@
         <v>505</v>
       </c>
       <c r="B507" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D507">
         <v>3</v>
@@ -12012,7 +12014,7 @@
         <v>506</v>
       </c>
       <c r="B508" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D508">
         <v>3</v>
@@ -12032,7 +12034,7 @@
         <v>507</v>
       </c>
       <c r="B509" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D509">
         <v>3</v>
@@ -12052,7 +12054,7 @@
         <v>508</v>
       </c>
       <c r="B510" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D510">
         <v>2</v>
@@ -12072,7 +12074,7 @@
         <v>509</v>
       </c>
       <c r="B511" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D511">
         <v>2</v>
@@ -12092,7 +12094,7 @@
         <v>510</v>
       </c>
       <c r="B512" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D512">
         <v>4</v>
@@ -12112,7 +12114,7 @@
         <v>511</v>
       </c>
       <c r="B513" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D513">
         <v>3</v>
@@ -12132,7 +12134,7 @@
         <v>512</v>
       </c>
       <c r="B514" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C514">
         <v>2</v>
@@ -12149,7 +12151,7 @@
         <v>513</v>
       </c>
       <c r="B515" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D515">
         <v>1</v>
@@ -12169,7 +12171,7 @@
         <v>514</v>
       </c>
       <c r="B516" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D516">
         <v>1</v>
@@ -12189,7 +12191,7 @@
         <v>515</v>
       </c>
       <c r="B517" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D517">
         <v>3</v>
@@ -12209,7 +12211,7 @@
         <v>516</v>
       </c>
       <c r="B518" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D518">
         <v>4</v>
@@ -12229,7 +12231,7 @@
         <v>517</v>
       </c>
       <c r="B519" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D519">
         <v>1</v>
@@ -12249,7 +12251,7 @@
         <v>518</v>
       </c>
       <c r="B520" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="D520">
         <v>4</v>
@@ -12269,7 +12271,7 @@
         <v>519</v>
       </c>
       <c r="B521" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C521">
         <v>4</v>
@@ -12286,7 +12288,7 @@
         <v>520</v>
       </c>
       <c r="B522" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D522">
         <v>1</v>
@@ -12306,7 +12308,7 @@
         <v>521</v>
       </c>
       <c r="B523" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D523">
         <v>2</v>
@@ -12326,7 +12328,7 @@
         <v>522</v>
       </c>
       <c r="B524" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C524">
         <v>2</v>
@@ -12343,7 +12345,7 @@
         <v>523</v>
       </c>
       <c r="B525" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C525">
         <v>2</v>
@@ -12360,7 +12362,7 @@
         <v>524</v>
       </c>
       <c r="B526" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C526">
         <v>3</v>
@@ -12377,7 +12379,7 @@
         <v>525</v>
       </c>
       <c r="B527" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C527">
         <v>3</v>
@@ -12394,7 +12396,7 @@
         <v>526</v>
       </c>
       <c r="B528" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D528">
         <v>3</v>
@@ -12414,7 +12416,7 @@
         <v>527</v>
       </c>
       <c r="B529" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C529">
         <v>2</v>
@@ -12431,7 +12433,7 @@
         <v>528</v>
       </c>
       <c r="B530" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D530">
         <v>3</v>
@@ -12451,7 +12453,7 @@
         <v>529</v>
       </c>
       <c r="B531" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D531">
         <v>2</v>
@@ -12471,7 +12473,7 @@
         <v>530</v>
       </c>
       <c r="B532" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C532">
         <v>2</v>
@@ -12488,7 +12490,7 @@
         <v>531</v>
       </c>
       <c r="B533" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D533">
         <v>3</v>
@@ -12508,7 +12510,7 @@
         <v>532</v>
       </c>
       <c r="B534" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D534">
         <v>2</v>

</xml_diff>